<commit_message>
Added Food, updated insurance
</commit_message>
<xml_diff>
--- a/Growth/RDDT_MODEL.xlsx
+++ b/Growth/RDDT_MODEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\Growth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE16C310-8B43-4C16-897B-F89908F80934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437C4DF9-E2AA-4825-BACD-5ED6B93FC2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19530" yWindow="0" windowWidth="18975" windowHeight="20985" activeTab="1" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="88">
   <si>
     <t>Price</t>
   </si>
@@ -285,6 +285,24 @@
   </si>
   <si>
     <t>275 to 285</t>
+  </si>
+  <si>
+    <t>666 analyst expectations</t>
+  </si>
+  <si>
+    <t>141% YOY</t>
+  </si>
+  <si>
+    <t>1 buillion in buybacks</t>
+  </si>
+  <si>
+    <t>595 to 605</t>
+  </si>
+  <si>
+    <t>210 to 220</t>
+  </si>
+  <si>
+    <t>Weak guidance</t>
   </si>
 </sst>
 </file>
@@ -296,13 +314,19 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -482,67 +506,73 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -887,141 +917,141 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="41" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="41"/>
+    <col min="1" max="1" width="19.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="39" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="39">
         <v>216</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="40">
         <v>45987</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5" s="39">
         <v>190</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="39" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="39">
         <f xml:space="preserve"> B4 * B5</f>
         <v>41040</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7" s="39">
         <v>2230</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="39">
         <v>25</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>11.75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9" s="39">
         <f>B6 - B7 + B8</f>
         <v>38835</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>13.78</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="41">
+      <c r="B11" s="39">
         <v>100.68</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="39">
         <v>61.7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="39">
         <v>21.7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="39">
         <v>15.86</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="39">
         <v>20.58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="41">
+      <c r="B17" s="39">
         <v>511.9</v>
       </c>
     </row>
@@ -1034,9 +1064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E38C8F-3B6A-4584-925C-61BD108C4B76}">
   <dimension ref="A1:V112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
       <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N72" sqref="N72"/>
+      <selection pane="topRight" activeCell="O73" sqref="O73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1050,7 +1080,7 @@
     <col min="11" max="11" width="14.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="1" customWidth="1"/>
     <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1156,6 +1186,9 @@
       <c r="N3" s="1">
         <v>585</v>
       </c>
+      <c r="O3" s="1">
+        <v>726</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
@@ -1194,6 +1227,9 @@
       <c r="N4" s="1">
         <v>480</v>
       </c>
+      <c r="O4" s="1">
+        <v>583</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -1231,6 +1267,9 @@
       </c>
       <c r="N5" s="1">
         <v>105</v>
+      </c>
+      <c r="O5" s="1">
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1289,8 +1328,7 @@
         <v>585</v>
       </c>
       <c r="O7" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>726</v>
       </c>
       <c r="P7" s="33">
         <f t="shared" si="1"/>
@@ -1340,7 +1378,9 @@
       <c r="N8" s="15">
         <v>52.5</v>
       </c>
-      <c r="O8" s="15"/>
+      <c r="O8" s="15">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="1:18" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1349,7 +1389,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <f t="shared" ref="D9:N9" si="2">D7 - SUM(D8:D8)</f>
+        <f t="shared" ref="D9:O9" si="2">D7 - SUM(D8:D8)</f>
         <v>136.69999999999999</v>
       </c>
       <c r="E9" s="3">
@@ -1391,6 +1431,10 @@
       <c r="N9" s="3">
         <f t="shared" si="2"/>
         <v>532.5</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" si="2"/>
+        <v>667</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1432,6 +1476,9 @@
       <c r="N10" s="1">
         <v>196.4</v>
       </c>
+      <c r="O10" s="1">
+        <v>198.9</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
@@ -1472,6 +1519,9 @@
       <c r="N11" s="1">
         <v>128.69999999999999</v>
       </c>
+      <c r="O11" s="1">
+        <v>163.9</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
@@ -1512,6 +1562,9 @@
       <c r="N12" s="1">
         <v>69</v>
       </c>
+      <c r="O12" s="1">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="1:18" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1564,7 +1617,7 @@
       </c>
       <c r="O13" s="3">
         <f t="shared" ref="O13" si="5">O9-SUM(O10:O12)</f>
-        <v>0</v>
+        <v>232.2</v>
       </c>
       <c r="P13" s="3">
         <f t="shared" ref="P13" si="6">P9-SUM(P10:P12)</f>
@@ -1612,6 +1665,9 @@
       <c r="N14" s="1">
         <v>161</v>
       </c>
+      <c r="O14" s="1">
+        <v>254.8</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
@@ -1650,6 +1706,9 @@
       <c r="N15" s="1">
         <v>2</v>
       </c>
+      <c r="O15" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:18" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
@@ -1700,8 +1759,7 @@
         <v>159</v>
       </c>
       <c r="O16" s="4">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="P16" s="4">
         <f t="shared" si="8"/>
@@ -1754,6 +1812,9 @@
       <c r="N17" s="1">
         <v>0.87</v>
       </c>
+      <c r="O17" s="1">
+        <v>1.32</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
@@ -1792,6 +1853,9 @@
       <c r="N18" s="1">
         <v>0.8</v>
       </c>
+      <c r="O18" s="1">
+        <v>1.24</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
@@ -1839,7 +1903,7 @@
       </c>
       <c r="O20" s="5">
         <f t="shared" ref="O20" si="11">(O7/K7) - 1</f>
-        <v>-1</v>
+        <v>0.69745148468552731</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" ref="P20" si="12">(P7/L7) - 1</f>
@@ -1858,7 +1922,7 @@
         <v>42</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" ref="E21:M21" si="14" xml:space="preserve"> (E7/D7) - 1</f>
+        <f t="shared" ref="E21:L21" si="14" xml:space="preserve"> (E7/D7) - 1</f>
         <v>0.11850946854001254</v>
       </c>
       <c r="F21" s="5">
@@ -1899,11 +1963,11 @@
       </c>
       <c r="O21" s="5">
         <f t="shared" si="15"/>
+        <v>0.24102564102564106</v>
+      </c>
+      <c r="P21" s="5">
+        <f t="shared" si="15"/>
         <v>-1</v>
-      </c>
-      <c r="P21" s="5" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
       </c>
       <c r="Q21" s="5" t="e">
         <f t="shared" si="15"/>
@@ -1958,6 +2022,9 @@
       <c r="N23" s="35">
         <v>0.91</v>
       </c>
+      <c r="O23" s="35">
+        <v>0.91900000000000004</v>
+      </c>
     </row>
     <row r="24" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="35" t="s">
@@ -1996,6 +2063,9 @@
       <c r="N24" s="35">
         <v>0.27800000000000002</v>
       </c>
+      <c r="O24" s="35">
+        <v>0.34699999999999998</v>
+      </c>
     </row>
     <row r="25" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="s">
@@ -2033,6 +2103,9 @@
       </c>
       <c r="N25" s="32">
         <v>236</v>
+      </c>
+      <c r="O25" s="32">
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:17" s="34" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2087,6 +2160,9 @@
         <f>SUM(N28:N29)</f>
         <v>116</v>
       </c>
+      <c r="O27" s="1">
+        <v>121.4</v>
+      </c>
     </row>
     <row r="28" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
@@ -2125,6 +2201,9 @@
       <c r="N28" s="1">
         <v>51.6</v>
       </c>
+      <c r="O28" s="1">
+        <v>52.5</v>
+      </c>
     </row>
     <row r="29" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
@@ -2163,6 +2242,9 @@
       <c r="N29" s="1">
         <v>64.400000000000006</v>
       </c>
+      <c r="O29" s="1">
+        <v>68.900000000000006</v>
+      </c>
     </row>
     <row r="30" spans="1:17" s="38" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
@@ -2213,7 +2295,7 @@
       </c>
       <c r="O30" s="38">
         <f t="shared" si="18"/>
-        <v>-1</v>
+        <v>0.19370698131760089</v>
       </c>
       <c r="P30" s="38">
         <f t="shared" si="18"/>
@@ -2270,7 +2352,7 @@
       </c>
       <c r="O31" s="38">
         <f t="shared" si="18"/>
-        <v>-1</v>
+        <v>9.375E-2</v>
       </c>
       <c r="P31" s="38">
         <f t="shared" si="18"/>
@@ -2327,7 +2409,7 @@
       </c>
       <c r="O32" s="38">
         <f t="shared" si="18"/>
-        <v>-1</v>
+        <v>0.28305400372439493</v>
       </c>
       <c r="P32" s="38">
         <f t="shared" si="18"/>
@@ -2390,6 +2472,9 @@
         <f>SUM(N35:N36)</f>
         <v>50.2</v>
       </c>
+      <c r="O34" s="1">
+        <v>50.7</v>
+      </c>
     </row>
     <row r="35" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
@@ -2428,6 +2513,9 @@
       <c r="N35" s="1">
         <v>23.1</v>
       </c>
+      <c r="O35" s="1">
+        <v>23</v>
+      </c>
     </row>
     <row r="36" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
@@ -2466,6 +2554,9 @@
       <c r="N36" s="1">
         <v>27.1</v>
       </c>
+      <c r="O36" s="1">
+        <v>27.7</v>
+      </c>
     </row>
     <row r="37" spans="1:17" s="38" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
@@ -2516,7 +2607,7 @@
       </c>
       <c r="O37" s="38">
         <f t="shared" si="22"/>
-        <v>-1</v>
+        <v>9.9783080260303914E-2</v>
       </c>
       <c r="P37" s="38">
         <f t="shared" si="22"/>
@@ -2560,7 +2651,7 @@
         <v>0.19170984455958551</v>
       </c>
       <c r="M38" s="38">
-        <f t="shared" ref="M38:N60" si="27">(M35/I35)-1</f>
+        <f t="shared" ref="M38:N59" si="27">(M35/I35)-1</f>
         <v>0.12254901960784315</v>
       </c>
       <c r="N38" s="38">
@@ -2569,7 +2660,7 @@
       </c>
       <c r="O38" s="38">
         <f t="shared" si="22"/>
-        <v>-1</v>
+        <v>5.0228310502283158E-2</v>
       </c>
       <c r="P38" s="38">
         <f t="shared" si="22"/>
@@ -2626,7 +2717,7 @@
       </c>
       <c r="O39" s="38">
         <f t="shared" si="22"/>
-        <v>-1</v>
+        <v>0.14462809917355379</v>
       </c>
       <c r="P39" s="38">
         <f t="shared" si="22"/>
@@ -2691,6 +2782,9 @@
         <f>SUM(N42:N43)</f>
         <v>65.8</v>
       </c>
+      <c r="O41" s="1">
+        <v>70.7</v>
+      </c>
     </row>
     <row r="42" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
@@ -2729,6 +2823,9 @@
       <c r="N42" s="1">
         <v>28.5</v>
       </c>
+      <c r="O42" s="1">
+        <v>29.5</v>
+      </c>
     </row>
     <row r="43" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
@@ -2767,6 +2864,9 @@
       <c r="N43" s="1">
         <v>37.299999999999997</v>
       </c>
+      <c r="O43" s="1">
+        <v>41.2</v>
+      </c>
     </row>
     <row r="44" spans="1:17" s="37" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="37" t="s">
@@ -2817,7 +2917,7 @@
       </c>
       <c r="O44" s="38">
         <f t="shared" si="35"/>
-        <v>-1</v>
+        <v>0.27158273381294973</v>
       </c>
       <c r="P44" s="38">
         <f t="shared" si="35"/>
@@ -2869,8 +2969,8 @@
         <v>6.7415730337078594E-2</v>
       </c>
       <c r="O45" s="38">
-        <f t="shared" ref="N45:P45" si="36">(O42/K42)-1</f>
-        <v>-1</v>
+        <f t="shared" ref="O45:P45" si="36">(O42/K42)-1</f>
+        <v>0.13026819923371646</v>
       </c>
       <c r="P45" s="38">
         <f t="shared" si="36"/>
@@ -2922,8 +3022,8 @@
         <v>0.41825095057034201</v>
       </c>
       <c r="O46" s="38">
-        <f t="shared" ref="N46:O46" si="37">(O43/K43)-1</f>
-        <v>-1</v>
+        <f t="shared" ref="O46" si="37">(O43/K43)-1</f>
+        <v>0.39661016949152561</v>
       </c>
       <c r="P46" s="38">
         <f>(P43/L43)-1</f>
@@ -2984,6 +3084,10 @@
         <f>SUM(N49:N50)</f>
         <v>443.8</v>
       </c>
+      <c r="O48" s="8">
+        <f>SUM(O49:O50)</f>
+        <v>471.6</v>
+      </c>
     </row>
     <row r="49" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
@@ -3022,6 +3126,9 @@
       <c r="N49" s="1">
         <v>187.8</v>
       </c>
+      <c r="O49" s="1">
+        <v>193.4</v>
+      </c>
     </row>
     <row r="50" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
@@ -3060,6 +3167,9 @@
       <c r="N50" s="1">
         <v>256</v>
       </c>
+      <c r="O50" s="1">
+        <v>278.2</v>
+      </c>
     </row>
     <row r="51" spans="1:17" s="37" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="37" t="s">
@@ -3105,12 +3215,12 @@
         <v>0.2164767747589833</v>
       </c>
       <c r="N51" s="38">
-        <f t="shared" ref="N51:N53" si="44">(N48/J48)-1</f>
+        <f t="shared" ref="N51" si="44">(N48/J48)-1</f>
         <v>0.21455938697318011</v>
       </c>
       <c r="O51" s="38">
         <f t="shared" ref="O51:O53" si="45">(O48/K48)-1</f>
-        <v>-1</v>
+        <v>0.2430152872957303</v>
       </c>
       <c r="P51" s="38">
         <f t="shared" ref="P51:P53" si="46">(P48/L48)-1</f>
@@ -3167,7 +3277,7 @@
       </c>
       <c r="O52" s="38">
         <f t="shared" si="45"/>
-        <v>-1</v>
+        <v>0.12311265969802565</v>
       </c>
       <c r="P52" s="38">
         <f t="shared" si="46"/>
@@ -3220,7 +3330,7 @@
       </c>
       <c r="O53" s="38">
         <f t="shared" si="45"/>
-        <v>-1</v>
+        <v>0.3426640926640927</v>
       </c>
       <c r="P53" s="38">
         <f t="shared" si="46"/>
@@ -3270,6 +3380,9 @@
       <c r="N55" s="1">
         <v>4.53</v>
       </c>
+      <c r="O55" s="1">
+        <v>5.98</v>
+      </c>
     </row>
     <row r="56" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
@@ -3308,6 +3421,9 @@
       <c r="N56" s="1">
         <v>9.0399999999999991</v>
       </c>
+      <c r="O56" s="1">
+        <v>10.79</v>
+      </c>
     </row>
     <row r="57" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
@@ -3346,6 +3462,9 @@
       <c r="N57" s="1">
         <v>1.84</v>
       </c>
+      <c r="O57" s="1">
+        <v>2.31</v>
+      </c>
     </row>
     <row r="58" spans="1:17" s="37" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A58" s="37" t="s">
@@ -3396,7 +3515,7 @@
       </c>
       <c r="O58" s="38">
         <f t="shared" ref="O58:O60" si="54">(O55/K55)-1</f>
-        <v>-1</v>
+        <v>0.42042755344418059</v>
       </c>
       <c r="P58" s="38">
         <f t="shared" ref="P58:P60" si="55">(P55/L55)-1</f>
@@ -3453,7 +3572,7 @@
       </c>
       <c r="O59" s="38">
         <f t="shared" si="54"/>
-        <v>-1</v>
+        <v>0.53267045454545436</v>
       </c>
       <c r="P59" s="38">
         <f t="shared" si="55"/>
@@ -3506,7 +3625,7 @@
       </c>
       <c r="O60" s="38">
         <f t="shared" si="54"/>
-        <v>-1</v>
+        <v>0.38323353293413187</v>
       </c>
       <c r="P60" s="38">
         <f t="shared" si="55"/>
@@ -3709,10 +3828,12 @@
       <c r="M70" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="N70" s="44" t="s">
+      <c r="N70" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="O70" s="10"/>
+      <c r="O70" s="45" t="s">
+        <v>85</v>
+      </c>
       <c r="P70" s="10"/>
       <c r="Q70" s="10"/>
       <c r="R70" s="10"/>
@@ -3726,15 +3847,24 @@
       <c r="M71" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="N71" s="41" t="s">
+      <c r="N71" s="47" t="s">
         <v>81</v>
+      </c>
+      <c r="O71" s="44" t="s">
+        <v>86</v>
       </c>
       <c r="V71" s="14"/>
     </row>
     <row r="72" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B72" s="13"/>
-      <c r="M72" s="43" t="s">
+      <c r="M72" s="41" t="s">
         <v>79</v>
+      </c>
+      <c r="N72" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="O72" s="44" t="s">
+        <v>87</v>
       </c>
       <c r="V72" s="14"/>
     </row>
@@ -3751,7 +3881,9 @@
       <c r="K73" s="17"/>
       <c r="L73" s="17"/>
       <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
+      <c r="N73" s="49">
+        <v>0.94</v>
+      </c>
       <c r="O73" s="17"/>
       <c r="P73" s="17"/>
       <c r="Q73" s="17"/>
@@ -3761,7 +3893,11 @@
       <c r="U73" s="17"/>
       <c r="V73" s="18"/>
     </row>
-    <row r="74" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N74" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="75" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B75" s="9" t="s">
         <v>36</v>
@@ -3777,8 +3913,10 @@
       <c r="K75" s="10"/>
       <c r="L75" s="10"/>
       <c r="M75" s="10"/>
-      <c r="N75" s="10"/>
-      <c r="O75" s="10"/>
+      <c r="N75" s="50"/>
+      <c r="O75" s="45" t="s">
+        <v>84</v>
+      </c>
       <c r="P75" s="10"/>
       <c r="Q75" s="10"/>
       <c r="R75" s="10"/>
@@ -3870,233 +4008,233 @@
     </row>
     <row r="89" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="13"/>
-      <c r="C89" s="39"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="39"/>
-      <c r="F89" s="39"/>
-      <c r="G89" s="39"/>
-      <c r="H89" s="39"/>
-      <c r="I89" s="39"/>
-      <c r="J89" s="39"/>
-      <c r="K89" s="39"/>
-      <c r="L89" s="39"/>
-      <c r="M89" s="39"/>
-      <c r="N89" s="39"/>
-      <c r="O89" s="39"/>
-      <c r="P89" s="39"/>
-      <c r="Q89" s="39"/>
-      <c r="R89" s="39"/>
-      <c r="S89" s="39"/>
-      <c r="T89" s="39"/>
-      <c r="U89" s="39"/>
-      <c r="V89" s="40"/>
+      <c r="C89" s="42"/>
+      <c r="D89" s="42"/>
+      <c r="E89" s="42"/>
+      <c r="F89" s="42"/>
+      <c r="G89" s="42"/>
+      <c r="H89" s="42"/>
+      <c r="I89" s="42"/>
+      <c r="J89" s="42"/>
+      <c r="K89" s="42"/>
+      <c r="L89" s="42"/>
+      <c r="M89" s="42"/>
+      <c r="N89" s="42"/>
+      <c r="O89" s="42"/>
+      <c r="P89" s="42"/>
+      <c r="Q89" s="42"/>
+      <c r="R89" s="42"/>
+      <c r="S89" s="42"/>
+      <c r="T89" s="42"/>
+      <c r="U89" s="42"/>
+      <c r="V89" s="43"/>
     </row>
     <row r="90" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="13"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="39"/>
-      <c r="F90" s="39"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="39"/>
-      <c r="I90" s="39"/>
-      <c r="J90" s="39"/>
-      <c r="K90" s="39"/>
-      <c r="L90" s="39"/>
-      <c r="M90" s="39"/>
-      <c r="N90" s="39"/>
-      <c r="O90" s="39"/>
-      <c r="P90" s="39"/>
-      <c r="Q90" s="39"/>
-      <c r="R90" s="39"/>
-      <c r="S90" s="39"/>
-      <c r="T90" s="39"/>
-      <c r="U90" s="39"/>
-      <c r="V90" s="40"/>
+      <c r="C90" s="42"/>
+      <c r="D90" s="42"/>
+      <c r="E90" s="42"/>
+      <c r="F90" s="42"/>
+      <c r="G90" s="42"/>
+      <c r="H90" s="42"/>
+      <c r="I90" s="42"/>
+      <c r="J90" s="42"/>
+      <c r="K90" s="42"/>
+      <c r="L90" s="42"/>
+      <c r="M90" s="42"/>
+      <c r="N90" s="42"/>
+      <c r="O90" s="42"/>
+      <c r="P90" s="42"/>
+      <c r="Q90" s="42"/>
+      <c r="R90" s="42"/>
+      <c r="S90" s="42"/>
+      <c r="T90" s="42"/>
+      <c r="U90" s="42"/>
+      <c r="V90" s="43"/>
     </row>
     <row r="91" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="13"/>
-      <c r="C91" s="39"/>
-      <c r="D91" s="39"/>
-      <c r="E91" s="39"/>
-      <c r="F91" s="39"/>
-      <c r="G91" s="39"/>
-      <c r="H91" s="39"/>
-      <c r="I91" s="39"/>
-      <c r="J91" s="39"/>
-      <c r="K91" s="39"/>
-      <c r="L91" s="39"/>
-      <c r="M91" s="39"/>
-      <c r="N91" s="39"/>
-      <c r="O91" s="39"/>
-      <c r="P91" s="39"/>
-      <c r="Q91" s="39"/>
-      <c r="R91" s="39"/>
-      <c r="S91" s="39"/>
-      <c r="T91" s="39"/>
-      <c r="U91" s="39"/>
-      <c r="V91" s="40"/>
+      <c r="C91" s="42"/>
+      <c r="D91" s="42"/>
+      <c r="E91" s="42"/>
+      <c r="F91" s="42"/>
+      <c r="G91" s="42"/>
+      <c r="H91" s="42"/>
+      <c r="I91" s="42"/>
+      <c r="J91" s="42"/>
+      <c r="K91" s="42"/>
+      <c r="L91" s="42"/>
+      <c r="M91" s="42"/>
+      <c r="N91" s="42"/>
+      <c r="O91" s="42"/>
+      <c r="P91" s="42"/>
+      <c r="Q91" s="42"/>
+      <c r="R91" s="42"/>
+      <c r="S91" s="42"/>
+      <c r="T91" s="42"/>
+      <c r="U91" s="42"/>
+      <c r="V91" s="43"/>
     </row>
     <row r="92" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="13"/>
-      <c r="C92" s="39"/>
-      <c r="D92" s="39"/>
-      <c r="E92" s="39"/>
-      <c r="F92" s="39"/>
-      <c r="G92" s="39"/>
-      <c r="H92" s="39"/>
-      <c r="I92" s="39"/>
-      <c r="J92" s="39"/>
-      <c r="K92" s="39"/>
-      <c r="L92" s="39"/>
-      <c r="M92" s="39"/>
-      <c r="N92" s="39"/>
-      <c r="O92" s="39"/>
-      <c r="P92" s="39"/>
-      <c r="Q92" s="39"/>
-      <c r="R92" s="39"/>
-      <c r="S92" s="39"/>
-      <c r="T92" s="39"/>
-      <c r="U92" s="39"/>
-      <c r="V92" s="40"/>
+      <c r="C92" s="42"/>
+      <c r="D92" s="42"/>
+      <c r="E92" s="42"/>
+      <c r="F92" s="42"/>
+      <c r="G92" s="42"/>
+      <c r="H92" s="42"/>
+      <c r="I92" s="42"/>
+      <c r="J92" s="42"/>
+      <c r="K92" s="42"/>
+      <c r="L92" s="42"/>
+      <c r="M92" s="42"/>
+      <c r="N92" s="42"/>
+      <c r="O92" s="42"/>
+      <c r="P92" s="42"/>
+      <c r="Q92" s="42"/>
+      <c r="R92" s="42"/>
+      <c r="S92" s="42"/>
+      <c r="T92" s="42"/>
+      <c r="U92" s="42"/>
+      <c r="V92" s="43"/>
     </row>
     <row r="93" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="13"/>
-      <c r="C93" s="39"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="39"/>
-      <c r="F93" s="39"/>
-      <c r="G93" s="39"/>
-      <c r="H93" s="39"/>
-      <c r="I93" s="39"/>
-      <c r="J93" s="39"/>
-      <c r="K93" s="39"/>
-      <c r="L93" s="39"/>
-      <c r="M93" s="39"/>
-      <c r="N93" s="39"/>
-      <c r="O93" s="39"/>
-      <c r="P93" s="39"/>
-      <c r="Q93" s="39"/>
-      <c r="R93" s="39"/>
-      <c r="S93" s="39"/>
-      <c r="T93" s="39"/>
-      <c r="U93" s="39"/>
-      <c r="V93" s="40"/>
+      <c r="C93" s="42"/>
+      <c r="D93" s="42"/>
+      <c r="E93" s="42"/>
+      <c r="F93" s="42"/>
+      <c r="G93" s="42"/>
+      <c r="H93" s="42"/>
+      <c r="I93" s="42"/>
+      <c r="J93" s="42"/>
+      <c r="K93" s="42"/>
+      <c r="L93" s="42"/>
+      <c r="M93" s="42"/>
+      <c r="N93" s="42"/>
+      <c r="O93" s="42"/>
+      <c r="P93" s="42"/>
+      <c r="Q93" s="42"/>
+      <c r="R93" s="42"/>
+      <c r="S93" s="42"/>
+      <c r="T93" s="42"/>
+      <c r="U93" s="42"/>
+      <c r="V93" s="43"/>
     </row>
     <row r="94" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="13"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
-      <c r="F94" s="39"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="39"/>
-      <c r="I94" s="39"/>
-      <c r="J94" s="39"/>
-      <c r="K94" s="39"/>
-      <c r="L94" s="39"/>
-      <c r="M94" s="39"/>
-      <c r="N94" s="39"/>
-      <c r="O94" s="39"/>
-      <c r="P94" s="39"/>
-      <c r="Q94" s="39"/>
-      <c r="R94" s="39"/>
-      <c r="S94" s="39"/>
-      <c r="T94" s="39"/>
-      <c r="U94" s="39"/>
-      <c r="V94" s="40"/>
+      <c r="C94" s="42"/>
+      <c r="D94" s="42"/>
+      <c r="E94" s="42"/>
+      <c r="F94" s="42"/>
+      <c r="G94" s="42"/>
+      <c r="H94" s="42"/>
+      <c r="I94" s="42"/>
+      <c r="J94" s="42"/>
+      <c r="K94" s="42"/>
+      <c r="L94" s="42"/>
+      <c r="M94" s="42"/>
+      <c r="N94" s="42"/>
+      <c r="O94" s="42"/>
+      <c r="P94" s="42"/>
+      <c r="Q94" s="42"/>
+      <c r="R94" s="42"/>
+      <c r="S94" s="42"/>
+      <c r="T94" s="42"/>
+      <c r="U94" s="42"/>
+      <c r="V94" s="43"/>
     </row>
     <row r="95" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="13"/>
-      <c r="C95" s="39"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="39"/>
-      <c r="F95" s="39"/>
-      <c r="G95" s="39"/>
-      <c r="H95" s="39"/>
-      <c r="I95" s="39"/>
-      <c r="J95" s="39"/>
-      <c r="K95" s="39"/>
-      <c r="L95" s="39"/>
-      <c r="M95" s="39"/>
-      <c r="N95" s="39"/>
-      <c r="O95" s="39"/>
-      <c r="P95" s="39"/>
-      <c r="Q95" s="39"/>
-      <c r="R95" s="39"/>
-      <c r="S95" s="39"/>
-      <c r="T95" s="39"/>
-      <c r="U95" s="39"/>
-      <c r="V95" s="40"/>
+      <c r="C95" s="42"/>
+      <c r="D95" s="42"/>
+      <c r="E95" s="42"/>
+      <c r="F95" s="42"/>
+      <c r="G95" s="42"/>
+      <c r="H95" s="42"/>
+      <c r="I95" s="42"/>
+      <c r="J95" s="42"/>
+      <c r="K95" s="42"/>
+      <c r="L95" s="42"/>
+      <c r="M95" s="42"/>
+      <c r="N95" s="42"/>
+      <c r="O95" s="42"/>
+      <c r="P95" s="42"/>
+      <c r="Q95" s="42"/>
+      <c r="R95" s="42"/>
+      <c r="S95" s="42"/>
+      <c r="T95" s="42"/>
+      <c r="U95" s="42"/>
+      <c r="V95" s="43"/>
     </row>
     <row r="96" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="13"/>
-      <c r="C96" s="39"/>
-      <c r="D96" s="39"/>
-      <c r="E96" s="39"/>
-      <c r="F96" s="39"/>
-      <c r="G96" s="39"/>
-      <c r="H96" s="39"/>
-      <c r="I96" s="39"/>
-      <c r="J96" s="39"/>
-      <c r="K96" s="39"/>
-      <c r="L96" s="39"/>
-      <c r="M96" s="39"/>
-      <c r="N96" s="39"/>
-      <c r="O96" s="39"/>
-      <c r="P96" s="39"/>
-      <c r="Q96" s="39"/>
-      <c r="R96" s="39"/>
-      <c r="S96" s="39"/>
-      <c r="T96" s="39"/>
-      <c r="U96" s="39"/>
-      <c r="V96" s="40"/>
+      <c r="C96" s="42"/>
+      <c r="D96" s="42"/>
+      <c r="E96" s="42"/>
+      <c r="F96" s="42"/>
+      <c r="G96" s="42"/>
+      <c r="H96" s="42"/>
+      <c r="I96" s="42"/>
+      <c r="J96" s="42"/>
+      <c r="K96" s="42"/>
+      <c r="L96" s="42"/>
+      <c r="M96" s="42"/>
+      <c r="N96" s="42"/>
+      <c r="O96" s="42"/>
+      <c r="P96" s="42"/>
+      <c r="Q96" s="42"/>
+      <c r="R96" s="42"/>
+      <c r="S96" s="42"/>
+      <c r="T96" s="42"/>
+      <c r="U96" s="42"/>
+      <c r="V96" s="43"/>
     </row>
     <row r="97" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="13"/>
-      <c r="C97" s="39"/>
-      <c r="D97" s="39"/>
-      <c r="E97" s="39"/>
-      <c r="F97" s="39"/>
-      <c r="G97" s="39"/>
-      <c r="H97" s="39"/>
-      <c r="I97" s="39"/>
-      <c r="J97" s="39"/>
-      <c r="K97" s="39"/>
-      <c r="L97" s="39"/>
-      <c r="M97" s="39"/>
-      <c r="N97" s="39"/>
-      <c r="O97" s="39"/>
-      <c r="P97" s="39"/>
-      <c r="Q97" s="39"/>
-      <c r="R97" s="39"/>
-      <c r="S97" s="39"/>
-      <c r="T97" s="39"/>
-      <c r="U97" s="39"/>
-      <c r="V97" s="40"/>
+      <c r="C97" s="42"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="42"/>
+      <c r="I97" s="42"/>
+      <c r="J97" s="42"/>
+      <c r="K97" s="42"/>
+      <c r="L97" s="42"/>
+      <c r="M97" s="42"/>
+      <c r="N97" s="42"/>
+      <c r="O97" s="42"/>
+      <c r="P97" s="42"/>
+      <c r="Q97" s="42"/>
+      <c r="R97" s="42"/>
+      <c r="S97" s="42"/>
+      <c r="T97" s="42"/>
+      <c r="U97" s="42"/>
+      <c r="V97" s="43"/>
     </row>
     <row r="98" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="13"/>
-      <c r="C98" s="39"/>
-      <c r="D98" s="39"/>
-      <c r="E98" s="39"/>
-      <c r="F98" s="39"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="39"/>
-      <c r="I98" s="39"/>
-      <c r="J98" s="39"/>
-      <c r="K98" s="39"/>
-      <c r="L98" s="39"/>
-      <c r="M98" s="39"/>
-      <c r="N98" s="39"/>
-      <c r="O98" s="39"/>
-      <c r="P98" s="39"/>
-      <c r="Q98" s="39"/>
-      <c r="R98" s="39"/>
-      <c r="S98" s="39"/>
-      <c r="T98" s="39"/>
-      <c r="U98" s="39"/>
-      <c r="V98" s="40"/>
+      <c r="C98" s="42"/>
+      <c r="D98" s="42"/>
+      <c r="E98" s="42"/>
+      <c r="F98" s="42"/>
+      <c r="G98" s="42"/>
+      <c r="H98" s="42"/>
+      <c r="I98" s="42"/>
+      <c r="J98" s="42"/>
+      <c r="K98" s="42"/>
+      <c r="L98" s="42"/>
+      <c r="M98" s="42"/>
+      <c r="N98" s="42"/>
+      <c r="O98" s="42"/>
+      <c r="P98" s="42"/>
+      <c r="Q98" s="42"/>
+      <c r="R98" s="42"/>
+      <c r="S98" s="42"/>
+      <c r="T98" s="42"/>
+      <c r="U98" s="42"/>
+      <c r="V98" s="43"/>
     </row>
     <row r="99" spans="2:22" ht="15" x14ac:dyDescent="0.25">
       <c r="B99" s="13"/>
@@ -4375,6 +4513,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C341BEE4C9A91F44BB4A4EF8E0A71E02" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db93f7cdcc50be3ddb7642c8d50e9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="878aac0c-df32-40a9-a231-d93e9c7b9b1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b63aaf3684aa43c37ed0cc1f5c2cf36e" ns3:_="">
     <xsd:import namespace="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
@@ -4518,22 +4671,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D266F6-4EBB-4FCE-8CE5-50B9641EB015}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4549,28 +4711,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>